<commit_message>
Updated with proper region info for National Grid
ITR data pipeline now properly uses ISO3166 to put countries in the correct regions (with the help of ESSD's UN region definitions).
</commit_message>
<xml_diff>
--- a/examples/data/rmi-20211120-output.xlsx
+++ b/examples/data/rmi-20211120-output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="157">
   <si>
     <t>company_name</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t>North America</t>
+  </si>
+  <si>
+    <t>Europe</t>
   </si>
   <si>
     <t>Electricity Utilities</t>
@@ -918,7 +921,7 @@
         <v>124</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H2">
         <v>15.292476505</v>
@@ -965,7 +968,7 @@
         <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H3">
         <v>6.490906199999998</v>
@@ -1012,7 +1015,7 @@
         <v>124</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H4">
         <v>5.314575956799998</v>
@@ -1053,7 +1056,7 @@
         <v>124</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H5">
         <v>20.5243372115</v>
@@ -1100,7 +1103,7 @@
         <v>124</v>
       </c>
       <c r="G6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H6">
         <v>35.41685299999996</v>
@@ -1147,13 +1150,13 @@
         <v>124</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H7">
         <v>83.96249309650005</v>
       </c>
       <c r="I7">
-        <v>58.13028231346648</v>
+        <v>58.13028231346649</v>
       </c>
       <c r="K7">
         <v>15561400000</v>
@@ -1194,7 +1197,7 @@
         <v>124</v>
       </c>
       <c r="G8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H8">
         <v>0.2335089999999994</v>
@@ -1241,7 +1244,7 @@
         <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H9">
         <v>7.614822899999996</v>
@@ -1288,7 +1291,7 @@
         <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H10">
         <v>17.02351533032852</v>
@@ -1335,7 +1338,7 @@
         <v>124</v>
       </c>
       <c r="G11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H11">
         <v>12.8612387470939</v>
@@ -1376,7 +1379,7 @@
         <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H12">
         <v>2.81985</v>
@@ -1423,7 +1426,7 @@
         <v>124</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H13">
         <v>39.19643799139996</v>
@@ -1470,7 +1473,7 @@
         <v>124</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H14">
         <v>97.78659735719998</v>
@@ -1517,7 +1520,7 @@
         <v>124</v>
       </c>
       <c r="G15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H15">
         <v>206.167169888941</v>
@@ -1564,7 +1567,7 @@
         <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H16">
         <v>10.528199334</v>
@@ -1611,7 +1614,7 @@
         <v>124</v>
       </c>
       <c r="G17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H17">
         <v>19.42686505303461</v>
@@ -1652,7 +1655,7 @@
         <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H18">
         <v>145.4066786083335</v>
@@ -1699,7 +1702,7 @@
         <v>124</v>
       </c>
       <c r="G19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H19">
         <v>48.2242056275</v>
@@ -1746,7 +1749,7 @@
         <v>124</v>
       </c>
       <c r="G20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H20">
         <v>0.06074384179999999</v>
@@ -1793,7 +1796,7 @@
         <v>124</v>
       </c>
       <c r="G21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H21">
         <v>19.2361809</v>
@@ -1840,7 +1843,7 @@
         <v>124</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H22">
         <v>12.92063789599999</v>
@@ -1881,7 +1884,7 @@
         <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H23">
         <v>4.294246499999999</v>
@@ -1922,10 +1925,10 @@
         <v>123</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H24">
         <v>3.890358999999996</v>
@@ -1969,7 +1972,7 @@
         <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H25">
         <v>1.2829038808</v>
@@ -2016,7 +2019,7 @@
         <v>124</v>
       </c>
       <c r="G26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H26">
         <v>15.98552608</v>
@@ -2057,7 +2060,7 @@
         <v>124</v>
       </c>
       <c r="G27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H27">
         <v>2.948309282</v>
@@ -2104,7 +2107,7 @@
         <v>124</v>
       </c>
       <c r="G28" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H28">
         <v>9.907384608500001</v>
@@ -2151,7 +2154,7 @@
         <v>124</v>
       </c>
       <c r="G29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H29">
         <v>33.15293172313432</v>
@@ -2198,7 +2201,7 @@
         <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H30">
         <v>27.00740443647359</v>
@@ -2245,7 +2248,7 @@
         <v>124</v>
       </c>
       <c r="G31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H31">
         <v>15.80069078849999</v>
@@ -2292,7 +2295,7 @@
         <v>124</v>
       </c>
       <c r="G32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H32">
         <v>53.45721600699997</v>
@@ -2339,7 +2342,7 @@
         <v>124</v>
       </c>
       <c r="G33" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H33">
         <v>1.263015</v>
@@ -2386,7 +2389,7 @@
         <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H34">
         <v>139.762091613559</v>
@@ -2433,7 +2436,7 @@
         <v>124</v>
       </c>
       <c r="G35" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H35">
         <v>16.113103994</v>
@@ -2480,7 +2483,7 @@
         <v>124</v>
       </c>
       <c r="G36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H36">
         <v>75.91699990534775</v>
@@ -2531,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1">
         <v>2019</v>
@@ -2641,7 +2644,7 @@
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E2">
         <v>11.994886356</v>
@@ -2751,7 +2754,7 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E3">
         <v>4.383048126</v>
@@ -2852,16 +2855,16 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2971,7 +2974,7 @@
         <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3081,7 +3084,7 @@
         <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E6">
         <v>11.081667744</v>
@@ -3191,7 +3194,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E7">
         <v>23.438028466</v>
@@ -3301,7 +3304,7 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E8">
         <v>67.605670319</v>
@@ -3313,7 +3316,7 @@
         <v>61.95792984199999</v>
       </c>
       <c r="H8">
-        <v>59.134059613</v>
+        <v>59.13405961300001</v>
       </c>
       <c r="I8">
         <v>56.310189375</v>
@@ -3328,7 +3331,7 @@
         <v>47.838578682</v>
       </c>
       <c r="M8">
-        <v>45.01470845200001</v>
+        <v>45.014708452</v>
       </c>
       <c r="N8">
         <v>42.190838217</v>
@@ -3364,7 +3367,7 @@
         <v>24.866829637</v>
       </c>
       <c r="Y8">
-        <v>23.40729612299999</v>
+        <v>23.407296123</v>
       </c>
       <c r="Z8">
         <v>21.947762609</v>
@@ -3402,16 +3405,16 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -3521,7 +3524,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E10">
         <v>0.025963092</v>
@@ -3631,7 +3634,7 @@
         <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3732,16 +3735,16 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E12">
         <v>2.860959944</v>
@@ -3842,16 +3845,16 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3961,7 +3964,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E14">
         <v>12.51296306</v>
@@ -4071,7 +4074,7 @@
         <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4181,7 +4184,7 @@
         <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E16">
         <v>1.202690405</v>
@@ -4282,16 +4285,16 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4401,7 +4404,7 @@
         <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E18">
         <v>27.00027425</v>
@@ -4511,7 +4514,7 @@
         <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E19">
         <v>31.432803556</v>
@@ -4583,7 +4586,7 @@
         <v>9.125652645000001</v>
       </c>
       <c r="AB19">
-        <v>8.111691240000001</v>
+        <v>8.111691239999999</v>
       </c>
       <c r="AC19">
         <v>7.097729835</v>
@@ -4595,7 +4598,7 @@
         <v>5.069807024</v>
       </c>
       <c r="AF19">
-        <v>4.05584562</v>
+        <v>4.055845619999999</v>
       </c>
       <c r="AG19">
         <v>3.041884214</v>
@@ -4621,7 +4624,7 @@
         <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E20">
         <v>83.595723119</v>
@@ -4731,7 +4734,7 @@
         <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4841,7 +4844,7 @@
         <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E22">
         <v>8.704698967000001</v>
@@ -4951,7 +4954,7 @@
         <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -5061,7 +5064,7 @@
         <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E24">
         <v>53.98120621</v>
@@ -5076,7 +5079,7 @@
         <v>49.994025891</v>
       </c>
       <c r="I24">
-        <v>48.585601716</v>
+        <v>48.58560171599999</v>
       </c>
       <c r="J24">
         <v>47.177177544</v>
@@ -5088,7 +5091,7 @@
         <v>44.360329198</v>
       </c>
       <c r="M24">
-        <v>42.95190502299999</v>
+        <v>42.951905023</v>
       </c>
       <c r="N24">
         <v>41.543480852</v>
@@ -5171,7 +5174,7 @@
         <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -5272,16 +5275,16 @@
     </row>
     <row r="26" spans="1:36">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -5391,7 +5394,7 @@
         <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27">
         <v>18.60611442</v>
@@ -5501,7 +5504,7 @@
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E28">
         <v>8.78796125</v>
@@ -5602,16 +5605,16 @@
     </row>
     <row r="29" spans="1:36">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E29">
         <v>3.979018143</v>
@@ -5721,7 +5724,7 @@
         <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -5831,7 +5834,7 @@
         <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E31">
         <v>2.427756991</v>
@@ -5941,7 +5944,7 @@
         <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E32">
         <v>1.991521434</v>
@@ -6051,7 +6054,7 @@
         <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E33">
         <v>10.09111576</v>
@@ -6161,7 +6164,7 @@
         <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E34">
         <v>2.604920783</v>
@@ -6271,7 +6274,7 @@
         <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E35">
         <v>5.367827989</v>
@@ -6381,7 +6384,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E36">
         <v>28.77891532</v>
@@ -6491,7 +6494,7 @@
         <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E37">
         <v>10.54957153</v>
@@ -6601,7 +6604,7 @@
         <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E38">
         <v>7.621927587</v>
@@ -6711,7 +6714,7 @@
         <v>116</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -6821,7 +6824,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E40">
         <v>0.495357536</v>
@@ -6931,7 +6934,7 @@
         <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E41">
         <v>63.436548403</v>
@@ -7032,16 +7035,16 @@
     </row>
     <row r="42" spans="1:36">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -7142,16 +7145,16 @@
     </row>
     <row r="43" spans="1:36">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -7261,7 +7264,7 @@
         <v>119</v>
       </c>
       <c r="D44" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E44">
         <v>9.874576585</v>
@@ -7371,7 +7374,7 @@
         <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E45">
         <v>43.15126858</v>
@@ -7494,7 +7497,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1">
         <v>2019</v>
@@ -7604,7 +7607,7 @@
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E2">
         <v>0.7077455691137845</v>
@@ -7714,7 +7717,7 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E3">
         <v>0.5203588779999999</v>
@@ -7815,16 +7818,16 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -7934,7 +7937,7 @@
         <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8044,7 +8047,7 @@
         <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E6">
         <v>0.4403657265077406</v>
@@ -8154,7 +8157,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E7">
         <v>0.64267691</v>
@@ -8264,16 +8267,16 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E8">
-        <v>0.6014097045624482</v>
+        <v>0.6014097045624481</v>
       </c>
       <c r="F8">
-        <v>0.57708224466243</v>
+        <v>0.5770822446624299</v>
       </c>
       <c r="G8">
-        <v>0.5527547847624117</v>
+        <v>0.5527547847624116</v>
       </c>
       <c r="H8">
         <v>0.5284657563085484</v>
@@ -8282,7 +8285,7 @@
         <v>0.5042152322039279</v>
       </c>
       <c r="J8">
-        <v>0.4800032845469086</v>
+        <v>0.4800032845469085</v>
       </c>
       <c r="K8">
         <v>0.4558299861001676</v>
@@ -8291,7 +8294,7 @@
         <v>0.4316954096569586</v>
       </c>
       <c r="M8">
-        <v>0.4075996272794525</v>
+        <v>0.4075996272794524</v>
       </c>
       <c r="N8">
         <v>0.3835427110191725</v>
@@ -8306,10 +8309,10 @@
         <v>0.322149032975004</v>
       </c>
       <c r="R8">
-        <v>0.308773855270523</v>
+        <v>0.3087738552705229</v>
       </c>
       <c r="S8">
-        <v>0.295420274656617</v>
+        <v>0.2954202746566169</v>
       </c>
       <c r="T8">
         <v>0.2820883300735705</v>
@@ -8321,10 +8324,10 @@
         <v>0.2554895103562274</v>
       </c>
       <c r="W8">
-        <v>0.2422227147158974</v>
+        <v>0.2422227147158975</v>
       </c>
       <c r="X8">
-        <v>0.2289777146550957</v>
+        <v>0.2289777146550956</v>
       </c>
       <c r="Y8">
         <v>0.2157545497809188</v>
@@ -8357,24 +8360,24 @@
         <v>0.09773517705967073</v>
       </c>
       <c r="AI8">
-        <v>0.08473253551185554</v>
+        <v>0.08473253551185553</v>
       </c>
       <c r="AJ8">
-        <v>0.07175216223412735</v>
+        <v>0.07175216223412734</v>
       </c>
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -8484,7 +8487,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E10">
         <v>0.02141957069165507</v>
@@ -8594,7 +8597,7 @@
         <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -8695,16 +8698,16 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E12">
         <v>0.4758590305010937</v>
@@ -8805,16 +8808,16 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -8924,7 +8927,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E14">
         <v>0.561341045</v>
@@ -9034,7 +9037,7 @@
         <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -9144,7 +9147,7 @@
         <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E16">
         <v>0.184867083</v>
@@ -9245,16 +9248,16 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:36">
@@ -9268,7 +9271,7 @@
         <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E18">
         <v>0.6716935589999999</v>
@@ -9378,7 +9381,7 @@
         <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E19">
         <v>0.3072671706007556</v>
@@ -9399,13 +9402,13 @@
         <v>0.2410583498091973</v>
       </c>
       <c r="K19">
-        <v>0.2286446119540666</v>
+        <v>0.2286446119540665</v>
       </c>
       <c r="L19">
         <v>0.2165167098480582</v>
       </c>
       <c r="M19">
-        <v>0.2046701014761142</v>
+        <v>0.2046701014761143</v>
       </c>
       <c r="N19">
         <v>0.1931002825222407</v>
@@ -9420,7 +9423,7 @@
         <v>0.1600071352238348</v>
       </c>
       <c r="R19">
-        <v>0.1495002497810018</v>
+        <v>0.1495002497810017</v>
       </c>
       <c r="S19">
         <v>0.1392482456118716</v>
@@ -9459,7 +9462,7 @@
         <v>0.04211087089281276</v>
       </c>
       <c r="AE19">
-        <v>0.03459747204870321</v>
+        <v>0.03459747204870322</v>
       </c>
       <c r="AF19">
         <v>0.02728692911139789</v>
@@ -9488,7 +9491,7 @@
         <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E20">
         <v>0.3838028685117988</v>
@@ -9598,7 +9601,7 @@
         <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -9708,7 +9711,7 @@
         <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E22">
         <v>0.404023942</v>
@@ -9818,7 +9821,7 @@
         <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -9928,16 +9931,16 @@
         <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E24">
-        <v>0.7113048472546465</v>
+        <v>0.7113048472546464</v>
       </c>
       <c r="F24">
         <v>0.6919162410599007</v>
       </c>
       <c r="G24">
-        <v>0.6725276348651549</v>
+        <v>0.672527634865155</v>
       </c>
       <c r="H24">
         <v>0.6531874430533254</v>
@@ -9949,7 +9952,7 @@
         <v>0.6146532802676916</v>
       </c>
       <c r="K24">
-        <v>0.5954597983104536</v>
+        <v>0.5954597983104537</v>
       </c>
       <c r="L24">
         <v>0.5763157076597147</v>
@@ -9964,13 +9967,13 @@
         <v>0.5191822220404967</v>
       </c>
       <c r="P24">
-        <v>0.5002381329846318</v>
+        <v>0.5002381329846319</v>
       </c>
       <c r="Q24">
         <v>0.4813446518568664</v>
       </c>
       <c r="R24">
-        <v>0.4625020212581998</v>
+        <v>0.4625020212581997</v>
       </c>
       <c r="S24">
         <v>0.4437104832026019</v>
@@ -9991,7 +9994,7 @@
         <v>0.3505276272409714</v>
       </c>
       <c r="Y24">
-        <v>0.3320477067070433</v>
+        <v>0.3320477067070432</v>
       </c>
       <c r="Z24">
         <v>0.3136205627240048</v>
@@ -10000,7 +10003,7 @@
         <v>0.2952464341158546</v>
       </c>
       <c r="AB24">
-        <v>0.2769255589638147</v>
+        <v>0.2769255589638148</v>
       </c>
       <c r="AC24">
         <v>0.2586581750909567</v>
@@ -10038,7 +10041,7 @@
         <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -10139,16 +10142,16 @@
     </row>
     <row r="26" spans="1:36">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -10258,7 +10261,7 @@
         <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27">
         <v>0.7071503386873526</v>
@@ -10368,7 +10371,7 @@
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E28">
         <v>0.5206077802825411</v>
@@ -10469,16 +10472,16 @@
     </row>
     <row r="29" spans="1:36">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E29">
         <v>0.49864586573088</v>
@@ -10588,7 +10591,7 @@
         <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -10698,7 +10701,7 @@
         <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E31">
         <v>0.3545481164133421</v>
@@ -10808,7 +10811,7 @@
         <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E32">
         <v>0.2997321612126735</v>
@@ -10918,7 +10921,7 @@
         <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E33">
         <v>0.5654922710000001</v>
@@ -11028,7 +11031,7 @@
         <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E34">
         <v>0.6042899100000001</v>
@@ -11138,7 +11141,7 @@
         <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E35">
         <v>0.4490472263533699</v>
@@ -11248,7 +11251,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E36">
         <v>0.8186775301020227</v>
@@ -11358,7 +11361,7 @@
         <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E37">
         <v>0.328743433</v>
@@ -11468,7 +11471,7 @@
         <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E38">
         <v>0.452991182</v>
@@ -11578,7 +11581,7 @@
         <v>116</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -11688,7 +11691,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E40">
         <v>0.070402124</v>
@@ -11798,7 +11801,7 @@
         <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E41">
         <v>0.4359009447400329</v>
@@ -11899,16 +11902,16 @@
     </row>
     <row r="42" spans="1:36">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -12009,16 +12012,16 @@
     </row>
     <row r="43" spans="1:36">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:36">
@@ -12032,7 +12035,7 @@
         <v>119</v>
       </c>
       <c r="D44" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E44">
         <v>0.5231776022639834</v>
@@ -12142,7 +12145,7 @@
         <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E45">
         <v>0.4625589852664037</v>
@@ -12265,7 +12268,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1">
         <v>2019</v>
@@ -12375,7 +12378,7 @@
         <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E2">
         <v>16.935348375</v>
@@ -12485,7 +12488,7 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E3">
         <v>8.421214907000001</v>
@@ -12586,16 +12589,16 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E4">
         <v>1.026422</v>
@@ -12705,7 +12708,7 @@
         <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E5">
         <v>6.367375351</v>
@@ -12815,7 +12818,7 @@
         <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E6">
         <v>25.16469173</v>
@@ -12925,7 +12928,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E7">
         <v>36.41700449</v>
@@ -13035,16 +13038,16 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E8">
-        <v>99.835176015</v>
+        <v>99.83517601499999</v>
       </c>
       <c r="F8">
         <v>99.91677389499999</v>
       </c>
       <c r="G8">
-        <v>99.99837177499998</v>
+        <v>99.998371775</v>
       </c>
       <c r="H8">
         <v>100.080204152</v>
@@ -13136,16 +13139,16 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E9">
         <v>0.000385</v>
@@ -13255,7 +13258,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E10">
         <v>1.212120114</v>
@@ -13365,7 +13368,7 @@
         <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E11">
         <v>9.613710092</v>
@@ -13466,16 +13469,16 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E12">
         <v>6.009696554999998</v>
@@ -13576,16 +13579,16 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E13">
         <v>2.786477</v>
@@ -13695,7 +13698,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E14">
         <v>22.28757311</v>
@@ -13805,7 +13808,7 @@
         <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E15">
         <v>13.86123875</v>
@@ -13915,7 +13918,7 @@
         <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E16">
         <v>6.505703404</v>
@@ -14016,16 +14019,16 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -14135,7 +14138,7 @@
         <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E18">
         <v>40.19730999</v>
@@ -14245,7 +14248,7 @@
         <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E19">
         <v>102.17303551</v>
@@ -14355,7 +14358,7 @@
         <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E20">
         <v>217.744885163</v>
@@ -14465,7 +14468,7 @@
         <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E21">
         <v>11.8010457</v>
@@ -14575,7 +14578,7 @@
         <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E22">
         <v>21.51489799</v>
@@ -14685,7 +14688,7 @@
         <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E23">
         <v>153.759110774</v>
@@ -14795,7 +14798,7 @@
         <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E24">
         <v>76.21933198999999</v>
@@ -14837,10 +14840,10 @@
         <v>77.52908060999999</v>
       </c>
       <c r="R24">
-        <v>77.64243719999999</v>
+        <v>77.6424372</v>
       </c>
       <c r="S24">
-        <v>77.75646796999999</v>
+        <v>77.75646797</v>
       </c>
       <c r="T24">
         <v>77.87117692</v>
@@ -14855,10 +14858,10 @@
         <v>78.21941336</v>
       </c>
       <c r="X24">
-        <v>78.33687563999999</v>
+        <v>78.33687564</v>
       </c>
       <c r="Y24">
-        <v>78.45503650999999</v>
+        <v>78.45503651</v>
       </c>
       <c r="Z24">
         <v>78.57390014000001</v>
@@ -14905,7 +14908,7 @@
         <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E25">
         <v>1.060753342</v>
@@ -15006,16 +15009,16 @@
     </row>
     <row r="26" spans="1:36">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E26">
         <v>16.139864776</v>
@@ -15125,7 +15128,7 @@
         <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E27">
         <v>26.311398565</v>
@@ -15235,7 +15238,7 @@
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E28">
         <v>16.840724204</v>
@@ -15336,16 +15339,16 @@
     </row>
     <row r="29" spans="1:36">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E29">
         <v>7.968699109999999</v>
@@ -15455,7 +15458,7 @@
         <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E30">
         <v>6.294009052000001</v>
@@ -15565,7 +15568,7 @@
         <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E31">
         <v>3.8916445</v>
@@ -15675,7 +15678,7 @@
         <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E32">
         <v>6.64332012</v>
@@ -15785,7 +15788,7 @@
         <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E33">
         <v>17.8415995</v>
@@ -15895,7 +15898,7 @@
         <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E34">
         <v>4.310335350000001</v>
@@ -16005,7 +16008,7 @@
         <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E35">
         <v>11.950171865</v>
@@ -16115,7 +16118,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E36">
         <v>35.15293172</v>
@@ -16225,7 +16228,7 @@
         <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E37">
         <v>31.981286</v>
@@ -16335,7 +16338,7 @@
         <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E38">
         <v>16.79911405</v>
@@ -16445,103 +16448,103 @@
         <v>116</v>
       </c>
       <c r="D39" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="F39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="G39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="H39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="I39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="J39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="K39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="L39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="M39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="N39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="O39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="P39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="Q39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="R39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="S39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="T39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="U39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="V39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="W39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="X39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="Y39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="Z39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AA39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AB39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AC39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AD39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AE39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AF39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AG39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AH39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AI39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
       <c r="AJ39">
-        <v>54.98742344999999</v>
+        <v>54.98742345</v>
       </c>
     </row>
     <row r="40" spans="1:36">
@@ -16555,7 +16558,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E40">
         <v>7.036116309</v>
@@ -16665,7 +16668,7 @@
         <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E41">
         <v>145.52973376</v>
@@ -16766,16 +16769,16 @@
     </row>
     <row r="42" spans="1:36">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E42">
         <v>1.248303</v>
@@ -16876,16 +16879,16 @@
     </row>
     <row r="43" spans="1:36">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -16995,7 +16998,7 @@
         <v>119</v>
       </c>
       <c r="D44" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E44">
         <v>18.87423399</v>
@@ -17105,7 +17108,7 @@
         <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E45">
         <v>93.200442563</v>

</xml_diff>